<commit_message>
Novas modificações e incremento
Novas modificações
</commit_message>
<xml_diff>
--- a/Matriz de Rastreabilidade/MR.xlsx
+++ b/Matriz de Rastreabilidade/MR.xlsx
@@ -16,52 +16,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
-    <t>Matriz de Rastreabilidade</t>
+    <t>ID</t>
   </si>
   <si>
-    <t>Menu</t>
-  </si>
-  <si>
-    <t>cor e imagem</t>
-  </si>
-  <si>
-    <t>receber notas</t>
-  </si>
-  <si>
-    <t>opções</t>
-  </si>
-  <si>
-    <t>repetir media</t>
-  </si>
-  <si>
-    <t>imprimir</t>
-  </si>
-  <si>
-    <t>RF</t>
-  </si>
-  <si>
-    <t>RNF:</t>
-  </si>
-  <si>
-    <t>Portabilidade</t>
-  </si>
-  <si>
-    <t>Interface</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Funcionalibilidade</t>
+    <t>R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,16 +36,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,12 +86,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,90 +412,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A2:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="I2" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>